<commit_message>
created test cases for auto connect module and executed test cases for general(settings)
</commit_message>
<xml_diff>
--- a/apps/features/backlog/desktop/windows/my account/my_account.xlsx
+++ b/apps/features/backlog/desktop/windows/my account/my_account.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\apps\features\backlog\desktop\windows\my account\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D5127F-3E7D-4D42-A112-686D0D58C9C1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98231C0B-6A9F-4F7A-8BDC-AF0EB95D5EBF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="91">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -364,6 +364,31 @@
   <si>
     <t>should be properly visible and properly working</t>
   </si>
+  <si>
+    <t>should performed well</t>
+  </si>
+  <si>
+    <t>check the the time taking for redirecting to
+previous page clicking back keyword</t>
+  </si>
+  <si>
+    <t>1. open the app store and install the symlexvpn app on your desktop device.
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. go to menubar
+5. tap to "my account"
+6. try to check the the time taking for redirecting to
+previous page clicking back keyword</t>
+  </si>
+  <si>
+    <t>should take less time</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>TC_SYM_MA_021</t>
+  </si>
 </sst>
 </file>
 
@@ -545,7 +570,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -575,14 +600,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -598,24 +615,28 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="57">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -805,6 +826,19 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1288,15 +1322,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:G23" headerRowDxfId="8" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:G24" headerRowDxfId="8" dataDxfId="7">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Test Case ID" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Prerequisites" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Title/Description" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Steps" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Expected result:" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Pass / Fail" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Comments" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Test Case ID" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Prerequisites" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Title/Description" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Steps" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Expected result:" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Pass / Fail" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Template-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1506,8 +1540,8 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <pane ySplit="3" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1523,15 +1557,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="13"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="21"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1553,13 +1587,13 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="16"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="24"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -1638,7 +1672,7 @@
       <c r="E4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G4" s="8" t="s">
@@ -1680,7 +1714,7 @@
       <c r="E5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G5" s="8" t="s">
@@ -1722,7 +1756,7 @@
       <c r="E6" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="F6" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G6" s="8" t="s">
@@ -1764,7 +1798,7 @@
       <c r="E7" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G7" s="8" t="s">
@@ -1806,7 +1840,7 @@
       <c r="E8" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="20" t="s">
+      <c r="F8" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G8" s="8" t="s">
@@ -1848,7 +1882,7 @@
       <c r="E9" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="F9" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G9" s="8" t="s">
@@ -1890,7 +1924,7 @@
       <c r="E10" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="20" t="s">
+      <c r="F10" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G10" s="8" t="s">
@@ -1932,7 +1966,7 @@
       <c r="E11" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="20" t="s">
+      <c r="F11" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G11" s="8" t="s">
@@ -1974,7 +2008,7 @@
       <c r="E12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="F12" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G12" s="8" t="s">
@@ -2007,7 +2041,7 @@
       <c r="B13" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="11" t="s">
         <v>32</v>
       </c>
       <c r="D13" s="8" t="s">
@@ -2016,7 +2050,7 @@
       <c r="E13" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="F13" s="20" t="s">
+      <c r="F13" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G13" s="8" t="s">
@@ -2043,23 +2077,23 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="12" t="s">
         <v>49</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="13" t="s">
         <v>50</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="F14" s="21"/>
-      <c r="G14" s="19"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="13"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -2081,23 +2115,23 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15" spans="1:26" ht="127.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="12" t="s">
         <v>53</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="13" t="s">
         <v>57</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="19"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="13"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -2119,23 +2153,23 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16" spans="1:26" ht="128.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="12" t="s">
         <v>54</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="12" t="s">
         <v>62</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="F16" s="21"/>
-      <c r="G16" s="19"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="13"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -2157,23 +2191,23 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="12" t="s">
         <v>55</v>
       </c>
       <c r="B17" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="13" t="s">
         <v>60</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="F17" s="21"/>
-      <c r="G17" s="19"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="13"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -2195,23 +2229,23 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="111" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="12" t="s">
         <v>56</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="13" t="s">
         <v>61</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="F18" s="21"/>
-      <c r="G18" s="19"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="13"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -2233,23 +2267,23 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="115.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="12" t="s">
         <v>67</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="13" t="s">
         <v>70</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="F19" s="21"/>
-      <c r="G19" s="19"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="13"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -2271,23 +2305,23 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="117" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="12" t="s">
         <v>68</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="13" t="s">
         <v>72</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="19"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="13"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -2309,23 +2343,23 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" ht="128.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="12" t="s">
         <v>69</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="13" t="s">
         <v>75</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="F21" s="21"/>
-      <c r="G21" s="19"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="13"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -2347,23 +2381,23 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="12" t="s">
         <v>78</v>
       </c>
       <c r="B22" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="13" t="s">
         <v>80</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="E22" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="F22" s="21"/>
-      <c r="G22" s="19"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="13"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -2385,21 +2419,23 @@
       <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="12" t="s">
         <v>79</v>
       </c>
       <c r="B23" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="13" t="s">
         <v>83</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="19"/>
+      <c r="E23" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F23" s="15"/>
+      <c r="G23" s="13"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -2420,14 +2456,26 @@
       <c r="Y23" s="1"/>
       <c r="Z23" s="1"/>
     </row>
-    <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="5"/>
+    <row r="24" spans="1:26" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="G24" s="17"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -29501,7 +29549,7 @@
     <mergeCell ref="A1:G2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4:F23" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4:F24" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Pass,Fail,N/A"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
created test cases for api_login_password_field and executed my account and forget pass module of symlex vpn
</commit_message>
<xml_diff>
--- a/apps/features/backlog/desktop/windows/my account/my_account.xlsx
+++ b/apps/features/backlog/desktop/windows/my account/my_account.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\apps\features\backlog\desktop\windows\my account\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98231C0B-6A9F-4F7A-8BDC-AF0EB95D5EBF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0B8A73-18E9-404D-92B5-154103892314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="98">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t>TC_SYM_MA_008</t>
-  </si>
-  <si>
-    <t>Need to show "Buy premium" instead of showing expiry date</t>
   </si>
   <si>
     <t>TC_SYM_MA_009</t>
@@ -164,9 +161,6 @@
 6. verify that the user's account details can be copied</t>
   </si>
   <si>
-    <t>user can copy their information</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. open the app store and install the symlexvpn app on your desktop device.
 2. open the installed symlexvpn application.
 3. login with proper credentials
@@ -215,18 +209,6 @@
     <t>check visibility of "My Account" section</t>
   </si>
   <si>
-    <t>verify that the "My Account" section is visible and 
-accessible from the home page after login</t>
-  </si>
-  <si>
-    <t>1. open the app store and install the symlexvpn app on your desktop device.
-2. open the installed symlexvpn application.
-3. login with proper credentials
-4. go to menubar
-5. tap to "my account"
-6. try to check the visibility of "My Account" section</t>
-  </si>
-  <si>
     <t>TC_SYM_MA_012</t>
   </si>
   <si>
@@ -237,9 +219,6 @@
   </si>
   <si>
     <t>TC_SYM_MA_015</t>
-  </si>
-  <si>
-    <t>check user profile information</t>
   </si>
   <si>
     <t>1. open the app store and install the symlexvpn app on your desktop device.
@@ -300,26 +279,7 @@
     <t>TC_SYM_MA_018</t>
   </si>
   <si>
-    <t>check lifetime vpn package</t>
-  </si>
-  <si>
-    <t>1. open the app store and install the symlexvpn app on your desktop device.
-2. open the installed symlexvpn application.
-3. login with proper credentials
-4. go to menubar
-5. tap to "my account"
-6. try to check lifetime vpn package</t>
-  </si>
-  <si>
     <t xml:space="preserve">check the back keyword </t>
-  </si>
-  <si>
-    <t>1. open the app store and install the symlexvpn app on your desktop device.
-2. open the installed symlexvpn application.
-3. login with proper credentials
-4. go to menubar
-5. tap to "my account"
-6. try to check the back keyword</t>
   </si>
   <si>
     <t>should redirect to previous page</t>
@@ -362,14 +322,94 @@
     <t>check the performance</t>
   </si>
   <si>
-    <t>should be properly visible and properly working</t>
-  </si>
-  <si>
     <t>should performed well</t>
   </si>
   <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>TC_SYM_MA_021</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Need to show "Buy premium" instead of showing expiry date and no expiry date is shown</t>
+  </si>
+  <si>
+    <t>1. open the app store and install the symlexvpn app on your desktop device.
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. go to menubar
+5. try to check the visibility of "My Account" section</t>
+  </si>
+  <si>
+    <t>verify that the "My Account" section is visible and 
+accessible from the menu page after login</t>
+  </si>
+  <si>
+    <t>check user profile information accurate displayed
+based on subscription status</t>
+  </si>
+  <si>
+    <t>check lifetime vpn package after clicking on it</t>
+  </si>
+  <si>
+    <t>check lifetime vpn package is properly visible as
+figma</t>
+  </si>
+  <si>
+    <t>1. open the app store and install the symlexvpn app on your desktop device.
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. go to menubar
+5. tap to "my account"
+6. try to check lifetime vpn package is properly visible as
+figma</t>
+  </si>
+  <si>
+    <t>1. open the app store and install the symlexvpn app on your desktop device.
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. go to menubar
+5. tap to "my account"
+6. try to check lifetime vpn package after clicking on it</t>
+  </si>
+  <si>
+    <t>should redirect to website checkout page</t>
+  </si>
+  <si>
+    <t>TC_SYM_MA_022</t>
+  </si>
+  <si>
+    <t>TC_SYM_MA_023</t>
+  </si>
+  <si>
+    <t>1. open the app store and install the symlexvpn app on your desktop device.
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. go to menubar
+5. tap to "my account"
+6. try to check by clicking back keyword</t>
+  </si>
+  <si>
+    <t>1. open the app store and install the symlexvpn app on your desktop device.
+2. open the installed symlexvpn application.
+3. login with proper credentials
+4. go to menubar
+5. tap to "my account"
+6. try to check the back keyword working properly while 
+connecting to server</t>
+  </si>
+  <si>
+    <t>should work properly and should take less time</t>
+  </si>
+  <si>
+    <t>check the back keyword working properly while not connecting to server</t>
+  </si>
+  <si>
     <t>check the the time taking for redirecting to
-previous page clicking back keyword</t>
+previous page clicking back keyword while connecting to server</t>
   </si>
   <si>
     <t>1. open the app store and install the symlexvpn app on your desktop device.
@@ -378,16 +418,10 @@
 4. go to menubar
 5. tap to "my account"
 6. try to check the the time taking for redirecting to
-previous page clicking back keyword</t>
+previous page clicking back keyword while connecting to server</t>
   </si>
   <si>
-    <t>should take less time</t>
-  </si>
-  <si>
-    <t>Fail</t>
-  </si>
-  <si>
-    <t>TC_SYM_MA_021</t>
+    <t>user can copy and paste their information</t>
   </si>
 </sst>
 </file>
@@ -450,12 +484,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -553,24 +587,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -600,38 +621,36 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,6 +668,21 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -676,7 +710,7 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -704,6 +738,7 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -731,6 +766,7 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -758,6 +794,7 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -785,6 +822,7 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -812,6 +850,7 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -826,19 +865,6 @@
           <color indexed="64"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1322,15 +1348,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:G24" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:G26" headerRowDxfId="8" dataDxfId="0">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Test Case ID" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Prerequisites" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Title/Description" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Steps" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Expected result:" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Pass / Fail" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Comments" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Test Case ID" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Prerequisites" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Title/Description" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Steps" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Expected result:" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Pass / Fail" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Comments" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="Template-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1537,11 +1563,11 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:Z990"/>
+  <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1557,15 +1583,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="21"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="15"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1587,13 +1613,13 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="22"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="24"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="18"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -1661,19 +1687,19 @@
         <v>9</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="14" t="s">
-        <v>7</v>
+      <c r="F4" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>8</v>
@@ -1703,19 +1729,19 @@
         <v>12</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>26</v>
+      <c r="E5" s="8" t="s">
+        <v>29</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>7</v>
+      <c r="F5" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>8</v>
@@ -1745,19 +1771,19 @@
         <v>13</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="E6" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>7</v>
+      <c r="F6" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>8</v>
@@ -1787,18 +1813,18 @@
         <v>14</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="11" t="s">
         <v>7</v>
       </c>
       <c r="G7" s="8" t="s">
@@ -1829,18 +1855,18 @@
         <v>15</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="11" t="s">
         <v>7</v>
       </c>
       <c r="G8" s="8" t="s">
@@ -1871,19 +1897,19 @@
         <v>16</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>39</v>
+        <v>97</v>
       </c>
-      <c r="F9" s="14" t="s">
-        <v>7</v>
+      <c r="F9" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>8</v>
@@ -1913,19 +1939,19 @@
         <v>17</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>7</v>
+      <c r="F10" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>8</v>
@@ -1955,18 +1981,18 @@
         <v>18</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="11" t="s">
         <v>7</v>
       </c>
       <c r="G11" s="8" t="s">
@@ -1994,22 +2020,22 @@
     </row>
     <row r="12" spans="1:26" ht="111.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>19</v>
+        <v>80</v>
       </c>
-      <c r="F12" s="14" t="s">
-        <v>7</v>
+      <c r="F12" s="11" t="s">
+        <v>79</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>8</v>
@@ -2036,21 +2062,21 @@
     </row>
     <row r="13" spans="1:26" ht="106.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>32</v>
+      <c r="C13" s="19" t="s">
+        <v>31</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="11" t="s">
         <v>7</v>
       </c>
       <c r="G13" s="8" t="s">
@@ -2076,24 +2102,26 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="1:26" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
-        <v>49</v>
+    <row r="14" spans="1:26" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>47</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="C14" s="13" t="s">
-        <v>50</v>
+      <c r="C14" s="8" t="s">
+        <v>48</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>52</v>
+        <v>81</v>
       </c>
-      <c r="E14" s="12" t="s">
-        <v>51</v>
+      <c r="E14" s="8" t="s">
+        <v>82</v>
       </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="13"/>
+      <c r="F14" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="8"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -2115,23 +2143,25 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15" spans="1:26" ht="127.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="8" t="s">
-        <v>24</v>
+      <c r="E15" s="8" t="s">
+        <v>54</v>
       </c>
-      <c r="C15" s="13" t="s">
-        <v>57</v>
+      <c r="F15" s="11" t="s">
+        <v>79</v>
       </c>
-      <c r="D15" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="F15" s="15"/>
-      <c r="G15" s="13"/>
+      <c r="G15" s="8"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -2153,23 +2183,25 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16" spans="1:26" ht="128.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="s">
-        <v>54</v>
+      <c r="A16" s="8" t="s">
+        <v>50</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>62</v>
+      <c r="C16" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
-      <c r="E16" s="13" t="s">
-        <v>64</v>
+      <c r="E16" s="8" t="s">
+        <v>59</v>
       </c>
-      <c r="F16" s="15"/>
-      <c r="G16" s="13"/>
+      <c r="F16" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="G16" s="8"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -2191,23 +2223,25 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="13" t="s">
+      <c r="D17" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>65</v>
+      <c r="E17" s="8" t="s">
+        <v>59</v>
       </c>
-      <c r="E17" s="13" t="s">
-        <v>64</v>
+      <c r="F17" s="11" t="s">
+        <v>79</v>
       </c>
-      <c r="F17" s="15"/>
-      <c r="G17" s="13"/>
+      <c r="G17" s="8"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -2229,23 +2263,25 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="111" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="13" t="s">
+      <c r="D18" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>66</v>
+      <c r="E18" s="8" t="s">
+        <v>59</v>
       </c>
-      <c r="E18" s="13" t="s">
-        <v>64</v>
+      <c r="F18" s="11" t="s">
+        <v>79</v>
       </c>
-      <c r="F18" s="15"/>
-      <c r="G18" s="13"/>
+      <c r="G18" s="8"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -2266,24 +2302,26 @@
       <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
     </row>
-    <row r="19" spans="1:26" ht="115.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="12" t="s">
-        <v>67</v>
+    <row r="19" spans="1:26" ht="127.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="C19" s="13" t="s">
-        <v>70</v>
+      <c r="C19" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
-      <c r="E19" s="13" t="s">
-        <v>84</v>
+      <c r="E19" s="8" t="s">
+        <v>59</v>
       </c>
-      <c r="F19" s="15"/>
-      <c r="G19" s="13"/>
+      <c r="F19" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="G19" s="8"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -2304,24 +2342,26 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" spans="1:26" ht="117" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="12" t="s">
-        <v>68</v>
+    <row r="20" spans="1:26" ht="108.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="C20" s="13" t="s">
-        <v>72</v>
+      <c r="C20" s="8" t="s">
+        <v>84</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
-      <c r="E20" s="13" t="s">
-        <v>74</v>
+      <c r="E20" s="12" t="s">
+        <v>88</v>
       </c>
-      <c r="F20" s="15"/>
-      <c r="G20" s="13"/>
+      <c r="F20" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="G20" s="12"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -2342,24 +2382,26 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26" ht="128.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="12" t="s">
-        <v>69</v>
+    <row r="21" spans="1:26" ht="111.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="8" t="s">
+        <v>64</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="C21" s="13" t="s">
-        <v>75</v>
+      <c r="C21" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
-      <c r="E21" s="13" t="s">
-        <v>76</v>
+      <c r="E21" s="8" t="s">
+        <v>66</v>
       </c>
-      <c r="F21" s="15"/>
-      <c r="G21" s="13"/>
+      <c r="F21" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="G21" s="8"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -2381,23 +2423,25 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="12" t="s">
-        <v>78</v>
+      <c r="A22" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="C22" s="13" t="s">
-        <v>80</v>
+      <c r="C22" s="8" t="s">
+        <v>94</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
-      <c r="E22" s="13" t="s">
-        <v>82</v>
+      <c r="E22" s="8" t="s">
+        <v>93</v>
       </c>
-      <c r="F22" s="15"/>
-      <c r="G22" s="13"/>
+      <c r="F22" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" s="12"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
@@ -2419,23 +2463,25 @@
       <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F23" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="F23" s="15"/>
-      <c r="G23" s="13"/>
+      <c r="G23" s="8"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -2457,25 +2503,25 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="16" t="s">
-        <v>90</v>
+      <c r="A24" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="C24" s="12" t="s">
-        <v>86</v>
+      <c r="C24" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
-      <c r="E24" s="17" t="s">
-        <v>88</v>
+      <c r="E24" s="8" t="s">
+        <v>74</v>
       </c>
-      <c r="F24" s="18" t="s">
-        <v>89</v>
+      <c r="F24" s="11" t="s">
+        <v>7</v>
       </c>
-      <c r="G24" s="17"/>
+      <c r="G24" s="8"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -2496,14 +2542,26 @@
       <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
     </row>
-    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="5"/>
+    <row r="25" spans="1:26" ht="123.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="G25" s="8"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
@@ -2524,14 +2582,26 @@
       <c r="Y25" s="1"/>
       <c r="Z25" s="1"/>
     </row>
-    <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="5"/>
+    <row r="26" spans="1:26" ht="141.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="G26" s="12"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
@@ -29544,12 +29614,30 @@
       <c r="Y990" s="1"/>
       <c r="Z990" s="1"/>
     </row>
+    <row r="991" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A991" s="5"/>
+      <c r="B991" s="5"/>
+      <c r="C991" s="5"/>
+      <c r="D991" s="5"/>
+      <c r="E991" s="5"/>
+      <c r="F991" s="6"/>
+      <c r="G991" s="5"/>
+    </row>
+    <row r="992" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A992" s="5"/>
+      <c r="B992" s="5"/>
+      <c r="C992" s="5"/>
+      <c r="D992" s="5"/>
+      <c r="E992" s="5"/>
+      <c r="F992" s="6"/>
+      <c r="G992" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4:F24" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4:F26" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Pass,Fail,N/A"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>